<commit_message>
viri in literatura, pregled del
</commit_message>
<xml_diff>
--- a/viri_literatura/pregled_del.xlsx
+++ b/viri_literatura/pregled_del.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nezakrzan/Documents/magisterska_naloga/viri_literatura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F191215-A119-E24F-AF2D-7822BD3D5C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B71BD6-07B2-5E4F-84CC-2897C6F52E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33080" yWindow="500" windowWidth="17640" windowHeight="21400" xr2:uid="{CB01C9AE-EC79-1343-B90F-0982167C6F7A}"/>
+    <workbookView xWindow="3680" yWindow="1160" windowWidth="36160" windowHeight="21400" xr2:uid="{CB01C9AE-EC79-1343-B90F-0982167C6F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>Avtorji</t>
   </si>
@@ -374,6 +374,9 @@
     <t>M. Lu,  Q. Zhao, K. L. Poston, E. V. Sullivan, A. Pfefferbaum, M. Shahid, M. Katz, L. M. Kouhsari, 
 K. Schulman, A. Milstein, J. C. Niebles, 
 V. W. Henderson</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -782,9 +785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BF311B-5A34-E442-BDA1-108848FF561F}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,6 +854,9 @@
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>

</xml_diff>